<commit_message>
Base de Datos Arreglada
Base_Datos_2001 y Base_Datos_2013
</commit_message>
<xml_diff>
--- a/Base de datos Python/base_datos_empleo.xlsx
+++ b/Base de datos Python/base_datos_empleo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Inestroza\Documents\GitHub\Proyecto_investigacion_semiario\Base de datos Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F22A31-D660-454E-85E6-BFA9E0B11824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BEC2F0-1AA8-4BAD-9697-BA7EA3B3B85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="831">
   <si>
     <t>Año</t>
   </si>
@@ -2511,6 +2511,18 @@
   </si>
   <si>
     <t xml:space="preserve">Calculo Ruido Blanco Poblacion Ocupados </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusion de laPrueba t-Students Poblacion Ocupada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">como la P(T&lt;=t)=0.000002&lt;0.05 y observamos que el </t>
+  </si>
+  <si>
+    <t xml:space="preserve">promedio de Hombres ocupados fue mayor que el </t>
+  </si>
+  <si>
+    <t xml:space="preserve">promedio de mujeres ocupadas </t>
   </si>
 </sst>
 </file>
@@ -2964,9 +2976,6 @@
     <xf numFmtId="165" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2979,10 +2988,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2997,22 +3018,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -16953,55 +16965,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="86" t="s">
         <v>540</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="84" t="s">
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="83" t="s">
         <v>544</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="84" t="s">
+      <c r="H1" s="83"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="83" t="s">
         <v>545</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="84" t="s">
+      <c r="K1" s="83"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="83" t="s">
         <v>546</v>
       </c>
-      <c r="N1" s="84"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="84" t="s">
+      <c r="N1" s="83"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="83" t="s">
         <v>547</v>
       </c>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="84" t="s">
+      <c r="Q1" s="83"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="83" t="s">
         <v>548</v>
       </c>
-      <c r="T1" s="84"/>
-      <c r="U1" s="85"/>
-      <c r="W1" s="83" t="s">
+      <c r="T1" s="83"/>
+      <c r="U1" s="84"/>
+      <c r="W1" s="87" t="s">
         <v>591</v>
       </c>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="1" t="s">
         <v>541</v>
       </c>
@@ -17287,11 +17299,11 @@
         <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="W5" s="83" t="s">
+      <c r="W5" s="87" t="s">
         <v>573</v>
       </c>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="83"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -17665,11 +17677,11 @@
         <f t="shared" si="5"/>
         <v>874</v>
       </c>
-      <c r="W10" s="83" t="s">
+      <c r="W10" s="87" t="s">
         <v>574</v>
       </c>
-      <c r="X10" s="83"/>
-      <c r="Y10" s="83"/>
+      <c r="X10" s="87"/>
+      <c r="Y10" s="87"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
@@ -18031,11 +18043,11 @@
         <f t="shared" si="5"/>
         <v>1117</v>
       </c>
-      <c r="W15" s="83" t="s">
+      <c r="W15" s="87" t="s">
         <v>575</v>
       </c>
-      <c r="X15" s="83"/>
-      <c r="Y15" s="83"/>
+      <c r="X15" s="87"/>
+      <c r="Y15" s="87"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -18409,11 +18421,11 @@
         <f t="shared" si="5"/>
         <v>3325</v>
       </c>
-      <c r="W20" s="83" t="s">
+      <c r="W20" s="87" t="s">
         <v>576</v>
       </c>
-      <c r="X20" s="83"/>
-      <c r="Y20" s="83"/>
+      <c r="X20" s="87"/>
+      <c r="Y20" s="87"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -18704,11 +18716,11 @@
         <f t="shared" si="5"/>
         <v>696</v>
       </c>
-      <c r="W24" s="83" t="s">
+      <c r="W24" s="87" t="s">
         <v>577</v>
       </c>
-      <c r="X24" s="83"/>
-      <c r="Y24" s="83"/>
+      <c r="X24" s="87"/>
+      <c r="Y24" s="87"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -19082,11 +19094,11 @@
         <f t="shared" si="5"/>
         <v>502</v>
       </c>
-      <c r="W29" s="83" t="s">
+      <c r="W29" s="87" t="s">
         <v>578</v>
       </c>
-      <c r="X29" s="83"/>
-      <c r="Y29" s="83"/>
+      <c r="X29" s="87"/>
+      <c r="Y29" s="87"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -19460,11 +19472,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W34" s="83" t="s">
+      <c r="W34" s="87" t="s">
         <v>579</v>
       </c>
-      <c r="X34" s="83"/>
-      <c r="Y34" s="83"/>
+      <c r="X34" s="87"/>
+      <c r="Y34" s="87"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -19838,11 +19850,11 @@
         <f t="shared" si="5"/>
         <v>161</v>
       </c>
-      <c r="W39" s="83" t="s">
+      <c r="W39" s="87" t="s">
         <v>580</v>
       </c>
-      <c r="X39" s="83"/>
-      <c r="Y39" s="83"/>
+      <c r="X39" s="87"/>
+      <c r="Y39" s="87"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -20204,11 +20216,11 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-      <c r="W44" s="83" t="s">
+      <c r="W44" s="87" t="s">
         <v>581</v>
       </c>
-      <c r="X44" s="83"/>
-      <c r="Y44" s="83"/>
+      <c r="X44" s="87"/>
+      <c r="Y44" s="87"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -20582,11 +20594,11 @@
         <f t="shared" si="5"/>
         <v>608</v>
       </c>
-      <c r="W49" s="83" t="s">
+      <c r="W49" s="87" t="s">
         <v>582</v>
       </c>
-      <c r="X49" s="83"/>
-      <c r="Y49" s="83"/>
+      <c r="X49" s="87"/>
+      <c r="Y49" s="87"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -20960,11 +20972,11 @@
         <f t="shared" si="5"/>
         <v>1725</v>
       </c>
-      <c r="W54" s="83" t="s">
+      <c r="W54" s="87" t="s">
         <v>583</v>
       </c>
-      <c r="X54" s="83"/>
-      <c r="Y54" s="83"/>
+      <c r="X54" s="87"/>
+      <c r="Y54" s="87"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -21338,11 +21350,11 @@
         <f t="shared" si="5"/>
         <v>712</v>
       </c>
-      <c r="W59" s="83" t="s">
+      <c r="W59" s="87" t="s">
         <v>584</v>
       </c>
-      <c r="X59" s="83"/>
-      <c r="Y59" s="83"/>
+      <c r="X59" s="87"/>
+      <c r="Y59" s="87"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -21716,11 +21728,11 @@
         <f t="shared" si="5"/>
         <v>92</v>
       </c>
-      <c r="W64" s="83" t="s">
+      <c r="W64" s="87" t="s">
         <v>585</v>
       </c>
-      <c r="X64" s="83"/>
-      <c r="Y64" s="83"/>
+      <c r="X64" s="87"/>
+      <c r="Y64" s="87"/>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65">
@@ -22082,11 +22094,11 @@
         <f t="shared" si="5"/>
         <v>45217</v>
       </c>
-      <c r="W69" s="83" t="s">
+      <c r="W69" s="87" t="s">
         <v>586</v>
       </c>
-      <c r="X69" s="83"/>
-      <c r="Y69" s="83"/>
+      <c r="X69" s="87"/>
+      <c r="Y69" s="87"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -22460,11 +22472,11 @@
         <f t="shared" si="15"/>
         <v>3591</v>
       </c>
-      <c r="W74" s="83" t="s">
+      <c r="W74" s="87" t="s">
         <v>587</v>
       </c>
-      <c r="X74" s="83"/>
-      <c r="Y74" s="83"/>
+      <c r="X74" s="87"/>
+      <c r="Y74" s="87"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75">
@@ -22838,11 +22850,11 @@
         <f t="shared" si="15"/>
         <v>11511</v>
       </c>
-      <c r="W79" s="83" t="s">
+      <c r="W79" s="87" t="s">
         <v>588</v>
       </c>
-      <c r="X79" s="83"/>
-      <c r="Y79" s="83"/>
+      <c r="X79" s="87"/>
+      <c r="Y79" s="87"/>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -23133,11 +23145,11 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-      <c r="W83" s="83" t="s">
+      <c r="W83" s="87" t="s">
         <v>589</v>
       </c>
-      <c r="X83" s="83"/>
-      <c r="Y83" s="83"/>
+      <c r="X83" s="87"/>
+      <c r="Y83" s="87"/>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -61942,6 +61954,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="W74:Y74"/>
+    <mergeCell ref="W79:Y79"/>
+    <mergeCell ref="W83:Y83"/>
+    <mergeCell ref="W49:Y49"/>
+    <mergeCell ref="W54:Y54"/>
+    <mergeCell ref="W59:Y59"/>
+    <mergeCell ref="W64:Y64"/>
+    <mergeCell ref="W69:Y69"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="W34:Y34"/>
+    <mergeCell ref="W39:Y39"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="W10:Y10"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="W20:Y20"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
@@ -61951,24 +61981,6 @@
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="W10:Y10"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="W20:Y20"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="W34:Y34"/>
-    <mergeCell ref="W39:Y39"/>
-    <mergeCell ref="W44:Y44"/>
-    <mergeCell ref="W74:Y74"/>
-    <mergeCell ref="W79:Y79"/>
-    <mergeCell ref="W83:Y83"/>
-    <mergeCell ref="W49:Y49"/>
-    <mergeCell ref="W54:Y54"/>
-    <mergeCell ref="W59:Y59"/>
-    <mergeCell ref="W64:Y64"/>
-    <mergeCell ref="W69:Y69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -61978,8 +61990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9444513-4619-48E8-BA10-92D760C4D8A9}">
   <dimension ref="A1:AX62"/>
   <sheetViews>
-    <sheetView topLeftCell="I18" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="Q20" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62015,39 +62027,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="87" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>551</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="86" t="s">
         <v>540</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="83" t="s">
         <v>544</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="84" t="s">
+      <c r="G2" s="83"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="83" t="s">
         <v>545</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="84" t="s">
+      <c r="J2" s="83"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="83" t="s">
         <v>546</v>
       </c>
-      <c r="M2" s="84"/>
-      <c r="N2" s="85"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="84"/>
       <c r="O2" s="19" t="s">
         <v>651</v>
       </c>
@@ -64197,8 +64209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85591A2D-7069-40DB-9539-955946B74862}">
   <dimension ref="A1:AX64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="N44" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64215,7 +64227,7 @@
     <col min="13" max="13" width="22.28515625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="15" max="15" width="52" customWidth="1"/>
-    <col min="16" max="16" width="27.7109375" customWidth="1"/>
+    <col min="16" max="16" width="49.42578125" customWidth="1"/>
     <col min="17" max="17" width="22.85546875" customWidth="1"/>
     <col min="18" max="18" width="44.85546875" customWidth="1"/>
     <col min="19" max="19" width="35.140625" customWidth="1"/>
@@ -64244,14 +64256,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="87" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -66217,6 +66229,9 @@
       <c r="AD49" s="58"/>
     </row>
     <row r="52" spans="16:34" x14ac:dyDescent="0.25">
+      <c r="P52" t="s">
+        <v>827</v>
+      </c>
       <c r="T52" s="50" t="s">
         <v>753</v>
       </c>
@@ -66241,6 +66256,9 @@
       <c r="AH52" s="79"/>
     </row>
     <row r="53" spans="16:34" x14ac:dyDescent="0.25">
+      <c r="P53" t="s">
+        <v>828</v>
+      </c>
       <c r="T53" s="53" t="s">
         <v>779</v>
       </c>
@@ -66257,6 +66275,9 @@
       <c r="AF53" s="54"/>
     </row>
     <row r="54" spans="16:34" x14ac:dyDescent="0.25">
+      <c r="P54" t="s">
+        <v>829</v>
+      </c>
       <c r="T54" s="53"/>
       <c r="U54" s="11"/>
       <c r="V54" s="11"/>
@@ -66277,6 +66298,9 @@
       <c r="AH54" s="28"/>
     </row>
     <row r="55" spans="16:34" x14ac:dyDescent="0.25">
+      <c r="P55" t="s">
+        <v>830</v>
+      </c>
       <c r="T55" s="45" t="s">
         <v>756</v>
       </c>
@@ -66598,8 +66622,8 @@
       <c r="A1" s="36"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -66607,9 +66631,9 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -66665,10 +66689,10 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="95" t="s">
         <v>611</v>
       </c>
-      <c r="C10" s="93"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="1"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -66694,48 +66718,48 @@
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="90" t="s">
+      <c r="B13" s="93" t="s">
         <v>605</v>
       </c>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="93" t="s">
         <v>604</v>
       </c>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="93" t="s">
         <v>606</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="92" t="s">
         <v>624</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
@@ -66747,30 +66771,30 @@
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="95" t="s">
+      <c r="I17" s="91" t="s">
         <v>616</v>
       </c>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
+      <c r="J17" s="91"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="91"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="35"/>
       <c r="C18" s="2">
         <v>2638033</v>
       </c>
-      <c r="E18" s="94" t="s">
+      <c r="E18" s="90" t="s">
         <v>614</v>
       </c>
-      <c r="F18" s="94"/>
+      <c r="F18" s="90"/>
       <c r="G18" s="12">
         <f>C23+C25</f>
         <v>2638033</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="2">
         <v>7332714</v>
       </c>
@@ -66807,12 +66831,12 @@
         <v>4694681</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="I21" s="95" t="s">
+      <c r="I21" s="91" t="s">
         <v>618</v>
       </c>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="95"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="91"/>
+      <c r="L21" s="91"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
@@ -66839,21 +66863,21 @@
       <c r="C25" s="2">
         <v>61872</v>
       </c>
-      <c r="I25" s="95" t="s">
+      <c r="I25" s="91" t="s">
         <v>621</v>
       </c>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="87" t="s">
         <v>632</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="13" t="s">
         <v>622</v>
       </c>
@@ -66870,10 +66894,10 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="87" t="s">
         <v>627</v>
       </c>
-      <c r="D28" s="83"/>
+      <c r="D28" s="87"/>
       <c r="E28" t="s">
         <v>629</v>
       </c>
@@ -66888,13 +66912,13 @@
       <c r="B29">
         <v>10</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="87" t="s">
         <v>633</v>
       </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30">
@@ -66912,15 +66936,15 @@
         <f>(G28/B29)*B30</f>
         <v>1500000</v>
       </c>
-      <c r="F31" s="83" t="s">
+      <c r="F31" s="87" t="s">
         <v>631</v>
       </c>
-      <c r="G31" s="83"/>
-      <c r="I31" s="83" t="s">
+      <c r="G31" s="87"/>
+      <c r="I31" s="87" t="s">
         <v>643</v>
       </c>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
+      <c r="J31" s="87"/>
+      <c r="K31" s="87"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
@@ -67023,23 +67047,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I21:L21"/>
     <mergeCell ref="I25:L25"/>
     <mergeCell ref="B16:H16"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -67074,12 +67098,12 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="94" t="s">
         <v>597</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -67087,24 +67111,24 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="94" t="s">
         <v>598</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="98" t="s">
         <v>592</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="9"/>
@@ -67113,10 +67137,10 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="98" t="s">
         <v>593</v>
       </c>
-      <c r="C6" s="97"/>
+      <c r="C6" s="98"/>
       <c r="D6" s="7"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -67126,10 +67150,10 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="98" t="s">
         <v>594</v>
       </c>
-      <c r="C7" s="97"/>
+      <c r="C7" s="98"/>
       <c r="D7" s="7"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -67139,10 +67163,10 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="97" t="s">
+      <c r="B8" s="98" t="s">
         <v>595</v>
       </c>
-      <c r="C8" s="97"/>
+      <c r="C8" s="98"/>
       <c r="D8" s="7"/>
       <c r="E8" s="1" t="s">
         <v>646</v>
@@ -67154,10 +67178,10 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="98" t="s">
         <v>596</v>
       </c>
-      <c r="C9" s="97"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="7" t="s">
         <v>609</v>
       </c>
@@ -67169,10 +67193,10 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="95" t="s">
         <v>610</v>
       </c>
-      <c r="C10" s="93"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="31" t="s">
         <v>611</v>
       </c>
@@ -67184,10 +67208,10 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="98" t="s">
         <v>599</v>
       </c>
-      <c r="C11" s="97"/>
+      <c r="C11" s="98"/>
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -67197,10 +67221,10 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="99" t="s">
         <v>600</v>
       </c>
-      <c r="C12" s="98"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -67214,66 +67238,66 @@
         <v>601</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="90" t="s">
+      <c r="D13" s="93" t="s">
         <v>605</v>
       </c>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="93"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="98" t="s">
         <v>602</v>
       </c>
-      <c r="C14" s="97"/>
-      <c r="D14" s="90" t="s">
+      <c r="C14" s="98"/>
+      <c r="D14" s="93" t="s">
         <v>604</v>
       </c>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="93"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="98" t="s">
         <v>603</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="90" t="s">
+      <c r="C15" s="98"/>
+      <c r="D15" s="93" t="s">
         <v>606</v>
       </c>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="93"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="92" t="s">
         <v>625</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96" t="s">
+      <c r="C16" s="92"/>
+      <c r="D16" s="92" t="s">
         <v>624</v>
       </c>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="96"/>
-      <c r="L16" s="95" t="s">
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="L16" s="91" t="s">
         <v>696</v>
       </c>
-      <c r="M16" s="95"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="91"/>
+      <c r="O16" s="91"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
@@ -67299,10 +67323,10 @@
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="97" t="s">
         <v>607</v>
       </c>
-      <c r="E19" s="99"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="4">
         <f>E21+E23</f>
         <v>1886435</v>
@@ -67316,12 +67340,12 @@
         <f>F19+E25</f>
         <v>4848916</v>
       </c>
-      <c r="L20" s="95" t="s">
+      <c r="L20" s="91" t="s">
         <v>698</v>
       </c>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="91"/>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
@@ -67545,6 +67569,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D13:J13"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="L20:O20"/>
@@ -67554,17 +67589,6 @@
     <mergeCell ref="D15:J15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:J16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
Código del Proyecto de Investigación
Código de los cálculos del Modelo AR(p) de diferentes ordenes.
</commit_message>
<xml_diff>
--- a/Base de datos Python/base_datos_empleo.xlsx
+++ b/Base de datos Python/base_datos_empleo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose Inestroza\Documents\GitHub\Proyecto_investigacion_semiario\Base de datos Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391B90E6-02FB-4AF6-A3B4-63890520D9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EC72EE-12D7-4466-9117-07C0FC313529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE DE DATOS 2001 Y 2013 MUNIC" sheetId="1" r:id="rId1"/>
@@ -3024,9 +3024,6 @@
     <xf numFmtId="165" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3039,10 +3036,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3057,22 +3066,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -17013,55 +17013,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="86" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="86" t="s">
         <v>540</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="84" t="s">
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="83" t="s">
         <v>544</v>
       </c>
-      <c r="H1" s="84"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="84" t="s">
+      <c r="H1" s="83"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="83" t="s">
         <v>545</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="84" t="s">
+      <c r="K1" s="83"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="83" t="s">
         <v>546</v>
       </c>
-      <c r="N1" s="84"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="84" t="s">
+      <c r="N1" s="83"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="83" t="s">
         <v>547</v>
       </c>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="84" t="s">
+      <c r="Q1" s="83"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="83" t="s">
         <v>548</v>
       </c>
-      <c r="T1" s="84"/>
-      <c r="U1" s="85"/>
-      <c r="W1" s="83" t="s">
+      <c r="T1" s="83"/>
+      <c r="U1" s="84"/>
+      <c r="W1" s="87" t="s">
         <v>591</v>
       </c>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
       <c r="D2" s="1" t="s">
         <v>541</v>
       </c>
@@ -17347,11 +17347,11 @@
         <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="W5" s="83" t="s">
+      <c r="W5" s="87" t="s">
         <v>573</v>
       </c>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="83"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -17725,11 +17725,11 @@
         <f t="shared" si="5"/>
         <v>874</v>
       </c>
-      <c r="W10" s="83" t="s">
+      <c r="W10" s="87" t="s">
         <v>574</v>
       </c>
-      <c r="X10" s="83"/>
-      <c r="Y10" s="83"/>
+      <c r="X10" s="87"/>
+      <c r="Y10" s="87"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
@@ -18091,11 +18091,11 @@
         <f t="shared" si="5"/>
         <v>1117</v>
       </c>
-      <c r="W15" s="83" t="s">
+      <c r="W15" s="87" t="s">
         <v>575</v>
       </c>
-      <c r="X15" s="83"/>
-      <c r="Y15" s="83"/>
+      <c r="X15" s="87"/>
+      <c r="Y15" s="87"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -18469,11 +18469,11 @@
         <f t="shared" si="5"/>
         <v>3325</v>
       </c>
-      <c r="W20" s="83" t="s">
+      <c r="W20" s="87" t="s">
         <v>576</v>
       </c>
-      <c r="X20" s="83"/>
-      <c r="Y20" s="83"/>
+      <c r="X20" s="87"/>
+      <c r="Y20" s="87"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -18764,11 +18764,11 @@
         <f t="shared" si="5"/>
         <v>696</v>
       </c>
-      <c r="W24" s="83" t="s">
+      <c r="W24" s="87" t="s">
         <v>577</v>
       </c>
-      <c r="X24" s="83"/>
-      <c r="Y24" s="83"/>
+      <c r="X24" s="87"/>
+      <c r="Y24" s="87"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -19142,11 +19142,11 @@
         <f t="shared" si="5"/>
         <v>502</v>
       </c>
-      <c r="W29" s="83" t="s">
+      <c r="W29" s="87" t="s">
         <v>578</v>
       </c>
-      <c r="X29" s="83"/>
-      <c r="Y29" s="83"/>
+      <c r="X29" s="87"/>
+      <c r="Y29" s="87"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -19520,11 +19520,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W34" s="83" t="s">
+      <c r="W34" s="87" t="s">
         <v>579</v>
       </c>
-      <c r="X34" s="83"/>
-      <c r="Y34" s="83"/>
+      <c r="X34" s="87"/>
+      <c r="Y34" s="87"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -19898,11 +19898,11 @@
         <f t="shared" si="5"/>
         <v>161</v>
       </c>
-      <c r="W39" s="83" t="s">
+      <c r="W39" s="87" t="s">
         <v>580</v>
       </c>
-      <c r="X39" s="83"/>
-      <c r="Y39" s="83"/>
+      <c r="X39" s="87"/>
+      <c r="Y39" s="87"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -20264,11 +20264,11 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-      <c r="W44" s="83" t="s">
+      <c r="W44" s="87" t="s">
         <v>581</v>
       </c>
-      <c r="X44" s="83"/>
-      <c r="Y44" s="83"/>
+      <c r="X44" s="87"/>
+      <c r="Y44" s="87"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -20642,11 +20642,11 @@
         <f t="shared" si="5"/>
         <v>608</v>
       </c>
-      <c r="W49" s="83" t="s">
+      <c r="W49" s="87" t="s">
         <v>582</v>
       </c>
-      <c r="X49" s="83"/>
-      <c r="Y49" s="83"/>
+      <c r="X49" s="87"/>
+      <c r="Y49" s="87"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -21020,11 +21020,11 @@
         <f t="shared" si="5"/>
         <v>1725</v>
       </c>
-      <c r="W54" s="83" t="s">
+      <c r="W54" s="87" t="s">
         <v>583</v>
       </c>
-      <c r="X54" s="83"/>
-      <c r="Y54" s="83"/>
+      <c r="X54" s="87"/>
+      <c r="Y54" s="87"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -21398,11 +21398,11 @@
         <f t="shared" si="5"/>
         <v>712</v>
       </c>
-      <c r="W59" s="83" t="s">
+      <c r="W59" s="87" t="s">
         <v>584</v>
       </c>
-      <c r="X59" s="83"/>
-      <c r="Y59" s="83"/>
+      <c r="X59" s="87"/>
+      <c r="Y59" s="87"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -21776,11 +21776,11 @@
         <f t="shared" si="5"/>
         <v>92</v>
       </c>
-      <c r="W64" s="83" t="s">
+      <c r="W64" s="87" t="s">
         <v>585</v>
       </c>
-      <c r="X64" s="83"/>
-      <c r="Y64" s="83"/>
+      <c r="X64" s="87"/>
+      <c r="Y64" s="87"/>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65">
@@ -22142,11 +22142,11 @@
         <f t="shared" si="5"/>
         <v>45217</v>
       </c>
-      <c r="W69" s="83" t="s">
+      <c r="W69" s="87" t="s">
         <v>586</v>
       </c>
-      <c r="X69" s="83"/>
-      <c r="Y69" s="83"/>
+      <c r="X69" s="87"/>
+      <c r="Y69" s="87"/>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -22520,11 +22520,11 @@
         <f t="shared" si="15"/>
         <v>3591</v>
       </c>
-      <c r="W74" s="83" t="s">
+      <c r="W74" s="87" t="s">
         <v>587</v>
       </c>
-      <c r="X74" s="83"/>
-      <c r="Y74" s="83"/>
+      <c r="X74" s="87"/>
+      <c r="Y74" s="87"/>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75">
@@ -22898,11 +22898,11 @@
         <f t="shared" si="15"/>
         <v>11511</v>
       </c>
-      <c r="W79" s="83" t="s">
+      <c r="W79" s="87" t="s">
         <v>588</v>
       </c>
-      <c r="X79" s="83"/>
-      <c r="Y79" s="83"/>
+      <c r="X79" s="87"/>
+      <c r="Y79" s="87"/>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -23193,11 +23193,11 @@
         <f t="shared" si="15"/>
         <v>12</v>
       </c>
-      <c r="W83" s="83" t="s">
+      <c r="W83" s="87" t="s">
         <v>589</v>
       </c>
-      <c r="X83" s="83"/>
-      <c r="Y83" s="83"/>
+      <c r="X83" s="87"/>
+      <c r="Y83" s="87"/>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -62002,6 +62002,24 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="W74:Y74"/>
+    <mergeCell ref="W79:Y79"/>
+    <mergeCell ref="W83:Y83"/>
+    <mergeCell ref="W49:Y49"/>
+    <mergeCell ref="W54:Y54"/>
+    <mergeCell ref="W59:Y59"/>
+    <mergeCell ref="W64:Y64"/>
+    <mergeCell ref="W69:Y69"/>
+    <mergeCell ref="W24:Y24"/>
+    <mergeCell ref="W29:Y29"/>
+    <mergeCell ref="W34:Y34"/>
+    <mergeCell ref="W39:Y39"/>
+    <mergeCell ref="W44:Y44"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="W10:Y10"/>
+    <mergeCell ref="W15:Y15"/>
+    <mergeCell ref="W20:Y20"/>
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:R1"/>
     <mergeCell ref="S1:U1"/>
@@ -62011,24 +62029,6 @@
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="W10:Y10"/>
-    <mergeCell ref="W15:Y15"/>
-    <mergeCell ref="W20:Y20"/>
-    <mergeCell ref="W24:Y24"/>
-    <mergeCell ref="W29:Y29"/>
-    <mergeCell ref="W34:Y34"/>
-    <mergeCell ref="W39:Y39"/>
-    <mergeCell ref="W44:Y44"/>
-    <mergeCell ref="W74:Y74"/>
-    <mergeCell ref="W79:Y79"/>
-    <mergeCell ref="W83:Y83"/>
-    <mergeCell ref="W49:Y49"/>
-    <mergeCell ref="W54:Y54"/>
-    <mergeCell ref="W59:Y59"/>
-    <mergeCell ref="W64:Y64"/>
-    <mergeCell ref="W69:Y69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -62038,7 +62038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9444513-4619-48E8-BA10-92D760C4D8A9}">
   <dimension ref="A1:AX64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -62075,39 +62075,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="87" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>551</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="86" t="s">
         <v>540</v>
       </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="83" t="s">
         <v>544</v>
       </c>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="84" t="s">
+      <c r="G2" s="83"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="83" t="s">
         <v>545</v>
       </c>
-      <c r="J2" s="84"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="84" t="s">
+      <c r="J2" s="83"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="83" t="s">
         <v>546</v>
       </c>
-      <c r="M2" s="84"/>
-      <c r="N2" s="85"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="84"/>
       <c r="O2" s="19" t="s">
         <v>651</v>
       </c>
@@ -64298,7 +64298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85591A2D-7069-40DB-9539-955946B74862}">
   <dimension ref="A1:AX64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N30" workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
@@ -64345,14 +64345,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="87" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -66717,7 +66717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2178D-C3AD-4559-BBBE-C65524D756B6}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B8" workbookViewId="0">
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
@@ -66733,8 +66733,8 @@
       <c r="A1" s="36"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -66742,9 +66742,9 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -66800,10 +66800,10 @@
       <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="95" t="s">
         <v>611</v>
       </c>
-      <c r="C10" s="93"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="1"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -66829,48 +66829,48 @@
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="90" t="s">
+      <c r="B13" s="93" t="s">
         <v>605</v>
       </c>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="93" t="s">
         <v>604</v>
       </c>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="90" t="s">
+      <c r="B15" s="93" t="s">
         <v>606</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="92" t="s">
         <v>624</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
@@ -66882,30 +66882,30 @@
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="95" t="s">
+      <c r="I17" s="91" t="s">
         <v>616</v>
       </c>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
+      <c r="J17" s="91"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="91"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="35"/>
       <c r="C18" s="2">
         <v>2638033</v>
       </c>
-      <c r="E18" s="94" t="s">
+      <c r="E18" s="90" t="s">
         <v>614</v>
       </c>
-      <c r="F18" s="94"/>
+      <c r="F18" s="90"/>
       <c r="G18" s="12">
         <f>C23+C25</f>
         <v>2638033</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="83"/>
-      <c r="C19" s="83"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="2">
         <v>7332714</v>
       </c>
@@ -66942,12 +66942,12 @@
         <v>4694681</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="I21" s="95" t="s">
+      <c r="I21" s="91" t="s">
         <v>618</v>
       </c>
-      <c r="J21" s="95"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="95"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="91"/>
+      <c r="L21" s="91"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
@@ -66974,21 +66974,21 @@
       <c r="C25" s="2">
         <v>61872</v>
       </c>
-      <c r="I25" s="95" t="s">
+      <c r="I25" s="91" t="s">
         <v>621</v>
       </c>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
+      <c r="J25" s="91"/>
+      <c r="K25" s="91"/>
+      <c r="L25" s="91"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="87" t="s">
         <v>632</v>
       </c>
-      <c r="D27" s="83"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="83"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
       <c r="I27" s="13" t="s">
         <v>622</v>
       </c>
@@ -67005,10 +67005,10 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="87" t="s">
         <v>627</v>
       </c>
-      <c r="D28" s="83"/>
+      <c r="D28" s="87"/>
       <c r="E28" t="s">
         <v>629</v>
       </c>
@@ -67023,13 +67023,13 @@
       <c r="B29">
         <v>10</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="87" t="s">
         <v>633</v>
       </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="83"/>
-      <c r="G29" s="83"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30">
@@ -67047,15 +67047,15 @@
         <f>(G28/B29)*B30</f>
         <v>1500000</v>
       </c>
-      <c r="F31" s="83" t="s">
+      <c r="F31" s="87" t="s">
         <v>631</v>
       </c>
-      <c r="G31" s="83"/>
-      <c r="I31" s="83" t="s">
+      <c r="G31" s="87"/>
+      <c r="I31" s="87" t="s">
         <v>643</v>
       </c>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
+      <c r="J31" s="87"/>
+      <c r="K31" s="87"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
@@ -67158,23 +67158,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I21:L21"/>
     <mergeCell ref="I25:L25"/>
     <mergeCell ref="B16:H16"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -67188,7 +67188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70861295-509C-42F1-98A7-F27B15B0F558}">
   <dimension ref="B2:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
@@ -67209,12 +67209,12 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="94" t="s">
         <v>597</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -67222,24 +67222,24 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="94" t="s">
         <v>598</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="98" t="s">
         <v>592</v>
       </c>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="9"/>
@@ -67248,10 +67248,10 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="98" t="s">
         <v>593</v>
       </c>
-      <c r="C6" s="97"/>
+      <c r="C6" s="98"/>
       <c r="D6" s="7"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -67261,10 +67261,10 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="98" t="s">
         <v>594</v>
       </c>
-      <c r="C7" s="97"/>
+      <c r="C7" s="98"/>
       <c r="D7" s="7"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -67274,10 +67274,10 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="97" t="s">
+      <c r="B8" s="98" t="s">
         <v>595</v>
       </c>
-      <c r="C8" s="97"/>
+      <c r="C8" s="98"/>
       <c r="D8" s="7"/>
       <c r="E8" s="1" t="s">
         <v>646</v>
@@ -67289,10 +67289,10 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="98" t="s">
         <v>596</v>
       </c>
-      <c r="C9" s="97"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="7" t="s">
         <v>609</v>
       </c>
@@ -67304,10 +67304,10 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="95" t="s">
         <v>610</v>
       </c>
-      <c r="C10" s="93"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="31" t="s">
         <v>611</v>
       </c>
@@ -67319,10 +67319,10 @@
       <c r="J10" s="9"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="98" t="s">
         <v>599</v>
       </c>
-      <c r="C11" s="97"/>
+      <c r="C11" s="98"/>
       <c r="D11" s="7"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -67332,10 +67332,10 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="99" t="s">
         <v>600</v>
       </c>
-      <c r="C12" s="98"/>
+      <c r="C12" s="99"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -67349,66 +67349,66 @@
         <v>601</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="D13" s="90" t="s">
+      <c r="D13" s="93" t="s">
         <v>605</v>
       </c>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
-      <c r="J13" s="90"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="93"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="98" t="s">
         <v>602</v>
       </c>
-      <c r="C14" s="97"/>
-      <c r="D14" s="90" t="s">
+      <c r="C14" s="98"/>
+      <c r="D14" s="93" t="s">
         <v>604</v>
       </c>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="93"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="98" t="s">
         <v>603</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="90" t="s">
+      <c r="C15" s="98"/>
+      <c r="D15" s="93" t="s">
         <v>606</v>
       </c>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="93"/>
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="93"/>
+      <c r="J15" s="93"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="92" t="s">
         <v>625</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96" t="s">
+      <c r="C16" s="92"/>
+      <c r="D16" s="92" t="s">
         <v>624</v>
       </c>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="96"/>
-      <c r="L16" s="95" t="s">
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="L16" s="91" t="s">
         <v>696</v>
       </c>
-      <c r="M16" s="95"/>
-      <c r="N16" s="95"/>
-      <c r="O16" s="95"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="91"/>
+      <c r="O16" s="91"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
@@ -67434,10 +67434,10 @@
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="99" t="s">
+      <c r="D19" s="97" t="s">
         <v>607</v>
       </c>
-      <c r="E19" s="99"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="4">
         <f>E21+E23</f>
         <v>1886435</v>
@@ -67451,12 +67451,12 @@
         <f>F19+E25</f>
         <v>4848916</v>
       </c>
-      <c r="L20" s="95" t="s">
+      <c r="L20" s="91" t="s">
         <v>698</v>
       </c>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="95"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="91"/>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
@@ -67680,6 +67680,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D13:J13"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="L16:O16"/>
     <mergeCell ref="L20:O20"/>
@@ -67689,17 +67700,6 @@
     <mergeCell ref="D15:J15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:J16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">

</xml_diff>